<commit_message>
header_row and tests complete
</commit_message>
<xml_diff>
--- a/tests/test_mentormatch.xlsx
+++ b/tests/test_mentormatch.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuki\projects\mentormatch\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\mentormatch\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F860DF4-AD14-4E2E-9C46-0DC4A55B9F4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3C7798-2234-425E-A35C-7C27A51AE816}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1416" yWindow="1272" windowWidth="21168" windowHeight="11088" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="mentors" sheetId="2" r:id="rId2"/>
     <sheet name="mentees" sheetId="3" r:id="rId3"/>
     <sheet name="test_applications" sheetId="4" r:id="rId4"/>
+    <sheet name="import_strings" sheetId="5" r:id="rId5"/>
+    <sheet name="find_header_row" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>hello</t>
   </si>
@@ -73,6 +75,33 @@
   </si>
   <si>
     <t>scitters</t>
+  </si>
+  <si>
+    <t>should_be_string</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  two spaces left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">two spaces right  </t>
+  </si>
+  <si>
+    <t>appl</t>
+  </si>
+  <si>
+    <t>grapes</t>
+  </si>
+  <si>
+    <t>ap</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>The answer should be 4!</t>
   </si>
 </sst>
 </file>
@@ -397,36 +426,36 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2/2</f>
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>_xlfn.CONCAT(A1, ", Jonathan")</f>
         <v>hello, Jonathan</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -444,9 +473,9 @@
       <selection activeCell="C5" sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -457,7 +486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -468,7 +497,7 @@
         <v>1732524</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -479,7 +508,7 @@
         <v>432436</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -490,7 +519,7 @@
         <v>423134</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -514,9 +543,9 @@
       <selection activeCell="B1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -536,13 +565,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ADF7BC-4D61-4B69-9FD5-BB55FF4CFF0C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -553,7 +582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -564,7 +593,7 @@
         <v>1732524</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -575,7 +604,7 @@
         <v>432436</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -586,7 +615,7 @@
         <v>423134</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -595,6 +624,100 @@
       </c>
       <c r="C5">
         <v>43243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767763AB-0C65-45CA-B5A2-51B6577CE94A}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303F9952-1526-4CDB-842E-6C7780915D3C}">
+  <dimension ref="K3:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tested all converters. About to implement wwid index
</commit_message>
<xml_diff>
--- a/tests/test_mentormatch.xlsx
+++ b/tests/test_mentormatch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\mentormatch\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D41BABC-332A-43C5-B319-C33FF0183474}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB661FFB-A973-4BF9-8793-FEE03940E7A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30750" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentors" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>hello</t>
   </si>
@@ -116,6 +116,39 @@
   </si>
   <si>
     <t>helper 30</t>
+  </si>
+  <si>
+    <t>tuple_ints</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>20 8</t>
+  </si>
+  <si>
+    <t>19twenty3</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>ints_with_missing</t>
+  </si>
+  <si>
+    <t>all_numbers</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>first_digit_missing</t>
+  </si>
+  <si>
+    <t>30 manager</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -151,9 +184,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,19 +634,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767763AB-0C65-45CA-B5A2-51B6577CE94A}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -622,8 +662,26 @@
       <c r="C1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -633,30 +691,84 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>457</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>1</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>63.5</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -664,21 +776,65 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>465</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>77557357</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>57</v>
+      </c>
+      <c r="G7">
+        <v>12541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -688,8 +844,26 @@
       <c r="C8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8">
+        <v>25.5</v>
+      </c>
+      <c r="H8">
+        <v>25.5</v>
+      </c>
+      <c r="I8">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -698,6 +872,53 @@
       </c>
       <c r="C9" t="s">
         <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9">
+        <v>858</v>
+      </c>
+      <c r="H9">
+        <v>858</v>
+      </c>
+      <c r="I9">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>43756</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43756</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43756</v>
+      </c>
+      <c r="E10" s="2">
+        <v>43756</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43756</v>
+      </c>
+      <c r="G10">
+        <v>23</v>
+      </c>
+      <c r="H10" s="2">
+        <v>43756</v>
+      </c>
+      <c r="I10" s="2">
+        <v>43756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented dtype check. still need to implement wwid index
</commit_message>
<xml_diff>
--- a/tests/test_mentormatch.xlsx
+++ b/tests/test_mentormatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\mentormatch\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB661FFB-A973-4BF9-8793-FEE03940E7A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B4AD14-0F73-4E91-B321-5FBDB8D1B34C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>hello</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>boolean_perfect</t>
   </si>
 </sst>
 </file>
@@ -634,10 +637,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767763AB-0C65-45CA-B5A2-51B6577CE94A}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G7" sqref="G7:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,12 +650,13 @@
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -672,16 +676,19 @@
         <v>31</v>
       </c>
       <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -700,7 +707,7 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2">
@@ -709,8 +716,11 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -729,17 +739,20 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -758,17 +771,20 @@
       <c r="F4" t="b">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>3</v>
       </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
       <c r="I4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -787,17 +803,20 @@
       <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>465</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
       </c>
       <c r="I5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -816,25 +835,31 @@
       <c r="F6" t="s">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>77557357</v>
       </c>
-      <c r="H6" t="s">
-        <v>0</v>
-      </c>
       <c r="I6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>57</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>12541</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -853,8 +878,8 @@
       <c r="F8" t="s">
         <v>28</v>
       </c>
-      <c r="G8">
-        <v>25.5</v>
+      <c r="G8" t="b">
+        <v>0</v>
       </c>
       <c r="H8">
         <v>25.5</v>
@@ -862,8 +887,11 @@
       <c r="I8">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -882,8 +910,8 @@
       <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="G9">
-        <v>858</v>
+      <c r="G9" t="b">
+        <v>0</v>
       </c>
       <c r="H9">
         <v>858</v>
@@ -891,8 +919,11 @@
       <c r="I9">
         <v>858</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43756</v>
       </c>
@@ -911,13 +942,16 @@
       <c r="F10" s="2">
         <v>43756</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>23</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>43756</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>43756</v>
       </c>
     </row>

</xml_diff>

<commit_message>
about to test drop_dups
</commit_message>
<xml_diff>
--- a/tests/test_mentormatch.xlsx
+++ b/tests/test_mentormatch.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\mentormatch\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EED58B-23E4-472D-ACFF-F291FEC37082}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D41CCD-AADB-403C-944F-E94228F4D677}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="699" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30750" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentors" sheetId="2" r:id="rId1"/>
     <sheet name="mentees" sheetId="3" r:id="rId2"/>
     <sheet name="test_index_names" sheetId="4" r:id="rId3"/>
-    <sheet name="test_converters" sheetId="5" r:id="rId4"/>
-    <sheet name="find_header_row" sheetId="6" r:id="rId5"/>
+    <sheet name="drop_dups" sheetId="7" r:id="rId4"/>
+    <sheet name="test_converters" sheetId="5" r:id="rId5"/>
+    <sheet name="find_header_row" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
   <si>
     <t>hello</t>
   </si>
@@ -152,6 +153,18 @@
   </si>
   <si>
     <t>boolean_perfect</t>
+  </si>
+  <si>
+    <t>I should</t>
+  </si>
+  <si>
+    <t>be removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I should </t>
+  </si>
+  <si>
+    <t>stay</t>
   </si>
 </sst>
 </file>
@@ -569,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ADF7BC-4D61-4B69-9FD5-BB55FF4CFF0C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +654,81 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2ED103-366B-4811-A01C-B5BA0C05633E}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>1732524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>43243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>423134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>43243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767763AB-0C65-45CA-B5A2-51B6577CE94A}">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -966,7 +1054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303F9952-1526-4CDB-842E-6C7780915D3C}">
   <dimension ref="K3:L5"/>
   <sheetViews>

</xml_diff>

<commit_message>
drop dups implemented and tested
</commit_message>
<xml_diff>
--- a/tests/test_mentormatch.xlsx
+++ b/tests/test_mentormatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\mentormatch\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D41CCD-AADB-403C-944F-E94228F4D677}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFA976B-36C1-4342-BCBC-EF638CA5BC41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30750" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -658,7 +658,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,24 +703,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C4">
-        <v>423134</v>
+        <v>43243</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>43243</v>
+        <v>423134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added header to mentor/mentee worksheets
</commit_message>
<xml_diff>
--- a/tests/test_mentormatch.xlsx
+++ b/tests/test_mentormatch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\mentormatch\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFA976B-36C1-4342-BCBC-EF638CA5BC41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEE7790-ADCB-497B-9EF5-88657FFEE790}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30750" yWindow="1950" windowWidth="21600" windowHeight="11385" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="699" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentors" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>hello</t>
   </si>
@@ -165,6 +165,45 @@
   </si>
   <si>
     <t>stay</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>position_level</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>genders_yes</t>
+  </si>
+  <si>
+    <t>sites_yes</t>
+  </si>
+  <si>
+    <t>sites_maybe</t>
+  </si>
+  <si>
+    <t>max_mentee_count</t>
+  </si>
+  <si>
+    <t>genders_maybe</t>
+  </si>
+  <si>
+    <t>preferred_wwids</t>
+  </si>
+  <si>
+    <t>wants_random_mentor</t>
+  </si>
+  <si>
+    <t>application_years</t>
+  </si>
+  <si>
+    <t>participation_years</t>
   </si>
 </sst>
 </file>
@@ -484,15 +523,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74385198-D54E-4AE5-817F-A59CEFD9899A}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -502,8 +551,35 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -514,7 +590,7 @@
         <v>1732524</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -525,7 +601,7 @@
         <v>432436</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -536,7 +612,7 @@
         <v>423134</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -554,15 +630,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2522D482-B94D-46FB-A9F8-A8684FBBFA17}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -571,6 +663,42 @@
       </c>
       <c r="C1" t="s">
         <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +711,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1048576"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2ED103-366B-4811-A01C-B5BA0C05633E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
implemented dynamic attributes for applicant
</commit_message>
<xml_diff>
--- a/tests/test_mentormatch.xlsx
+++ b/tests/test_mentormatch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\mentormatch\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB6B7BD-ED5C-492F-B1C5-FDEE0ACB5A4F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864626E2-54FE-40A9-95CD-A07FB6AE0144}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentors" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>hello</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>participation_years</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74385198-D54E-4AE5-817F-A59CEFD9899A}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -785,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2ED103-366B-4811-A01C-B5BA0C05633E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +812,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
added, then commented out the additional of new df cols
</commit_message>
<xml_diff>
--- a/tests/test_mentormatch.xlsx
+++ b/tests/test_mentormatch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\mentormatch\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuki\projects\mentormatch\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864626E2-54FE-40A9-95CD-A07FB6AE0144}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531239C8-CC94-45AD-AE80-E41A4FF376CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="2376" windowWidth="23256" windowHeight="12576" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentors" sheetId="2" r:id="rId1"/>
@@ -789,7 +789,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
i just realized that I can't store sequences in pandas... I think I'll try TinyDB
</commit_message>
<xml_diff>
--- a/tests/test_mentormatch.xlsx
+++ b/tests/test_mentormatch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuki\projects\mentormatch\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531239C8-CC94-45AD-AE80-E41A4FF376CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5B0338-F23B-4006-B8B5-2DC35306CF52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="2376" windowWidth="23256" windowHeight="12576" tabRatio="699" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="2376" windowWidth="23256" windowHeight="12576" tabRatio="699" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentors" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
   <si>
     <t>hello</t>
   </si>
@@ -207,6 +207,48 @@
   </si>
   <si>
     <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Johnny</t>
+  </si>
+  <si>
+    <t>Suzie</t>
+  </si>
+  <si>
+    <t>Timmy</t>
+  </si>
+  <si>
+    <t>Billy</t>
+  </si>
+  <si>
+    <t>Xavier</t>
+  </si>
+  <si>
+    <t>Petronella</t>
+  </si>
+  <si>
+    <t>Osgood</t>
+  </si>
+  <si>
+    <t>Nebuchadnezzar</t>
+  </si>
+  <si>
+    <t>Hannurabi</t>
+  </si>
+  <si>
+    <t>Babby</t>
+  </si>
+  <si>
+    <t>Nautilus</t>
+  </si>
+  <si>
+    <t>Jedediah</t>
+  </si>
+  <si>
+    <t>123, 456</t>
+  </si>
+  <si>
+    <t>123, 234, 345</t>
   </si>
 </sst>
 </file>
@@ -529,7 +571,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,46 +626,46 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="C2">
-        <v>1732524</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C3">
-        <v>432436</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C4">
-        <v>423134</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="C5">
-        <v>43243</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -633,10 +675,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2522D482-B94D-46FB-A9F8-A8684FBBFA17}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,6 +746,47 @@
         <v>55</v>
       </c>
     </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3">
+        <v>1234</v>
+      </c>
+      <c r="L3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4">
+        <v>1345</v>
+      </c>
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>1456</v>
+      </c>
+      <c r="L5" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -788,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2ED103-366B-4811-A01C-B5BA0C05633E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>